<commit_message>
Iterating and fixing numbers
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vodafone</t>
   </si>
 </sst>
 </file>
@@ -129,10 +132,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -164,6 +167,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>7422965940</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>